<commit_message>
added sizing study for VA
</commit_message>
<xml_diff>
--- a/projects/virginia/well_diameter_sweep/user_inputs.xlsx
+++ b/projects/virginia/well_diameter_sweep/user_inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1DCD3B-83E4-4DC1-A4DD-30B23DC4907E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC67DEA-FD21-4424-9FB1-94343BE86A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="low_k" sheetId="9" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -673,7 +673,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,7 +849,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -901,7 +901,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,7 +1077,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,7 +1305,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F724D3C2-5C34-4460-84ED-CEBDE5C6F692}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,7 +1533,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>5</v>

</xml_diff>